<commit_message>
category별로 Store instance 분류
</commit_message>
<xml_diff>
--- a/crawling/data/univ_addr.xlsx
+++ b/crawling/data/univ_addr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\error_fix\crawling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B4F695-AA88-462F-AD8B-BFD8A4579C58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4992D3EB-A6C9-44ED-943F-03AD00891023}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D29C7F78-80EF-4A9E-9CCC-5F37658D6B0A}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{D29C7F78-80EF-4A9E-9CCC-5F37658D6B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="110">
   <si>
     <t>강경욱</t>
   </si>
@@ -57,12 +57,6 @@
     <t xml:space="preserve"> 고려대학교</t>
   </si>
   <si>
-    <t>김대환</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 울산대학교</t>
-  </si>
-  <si>
     <t>김상현</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t xml:space="preserve"> 숙명여자대학교</t>
   </si>
   <si>
-    <t>신보라</t>
-  </si>
-  <si>
     <t>이수경</t>
   </si>
   <si>
@@ -387,14 +378,6 @@
   </si>
   <si>
     <t>경기도 용인시 처인구 모현읍 외대로 81</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>울산광역시 남구 대학로 93</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> ?!</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -783,7 +766,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -801,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75">
@@ -812,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75">
@@ -823,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75">
@@ -834,505 +817,492 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>

</xml_diff>